<commit_message>
different versions of models, incl. TotalCategory variables
</commit_message>
<xml_diff>
--- a/taxonomy.xlsx
+++ b/taxonomy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abeurope-my.sharepoint.com/personal/mattias_mutso_externi_cz/Documents/Documents/AsahiUK_MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1887" documentId="8_{89E4EC9A-90DE-43F4-9AC7-CA845E774634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E04BCF18-4E56-4E82-BF44-38D177E80EFA}"/>
+  <xr:revisionPtr revIDLastSave="1904" documentId="8_{89E4EC9A-90DE-43F4-9AC7-CA845E774634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{358638EF-8C09-42CE-BFB6-4331C3999890}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{76ACBFB2-FDB9-4F29-83E0-3CEBBBD05A87}"/>
   </bookViews>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18501" uniqueCount="2153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18731" uniqueCount="2203">
   <si>
     <t>variable_name</t>
   </si>
@@ -6557,6 +6557,156 @@
   </si>
   <si>
     <t>actuals</t>
+  </si>
+  <si>
+    <t>Total Category Level Data</t>
+  </si>
+  <si>
+    <t>cat_</t>
+  </si>
+  <si>
+    <t>volume multiples glass pack</t>
+  </si>
+  <si>
+    <t>volume multiples can pack</t>
+  </si>
+  <si>
+    <t>volume impulse glass pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_glass_single</t>
+  </si>
+  <si>
+    <t>vol_multiples_can_single</t>
+  </si>
+  <si>
+    <t>vol_impulse_glass_single</t>
+  </si>
+  <si>
+    <t>vol_impulse_can_single</t>
+  </si>
+  <si>
+    <t>vol_multiples_glass_2_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_glass_3_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_glass_4_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_glass_6_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_glass_8_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_glass_10_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_glass_12_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_glass_15_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_glass_18_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_glass_20_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_glass_24_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_can_2_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_can_4_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_can_6_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_can_8_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_can_10_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_can_12_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_can_15_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_can_18_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_can_20_pack</t>
+  </si>
+  <si>
+    <t>vol_multiples_can_24_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_glass_2_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_glass_3_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_glass_4_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_glass_5_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_glass_6_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_glass_10_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_glass_12_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_glass_15_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_glass_8_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_glass_18_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_glass_20_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_can_24_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_can_4_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_can_6_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_can_10_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_can_12_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_can_15_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_can_8_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_can_18_pack</t>
+  </si>
+  <si>
+    <t>vol_impulse_can_20_pack</t>
   </si>
 </sst>
 </file>
@@ -7017,11 +7167,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538DC1F5-E4A4-461E-8C87-E865C98C4EFC}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I2918"/>
+  <dimension ref="A1:I2964"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A747" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2919" sqref="H2919"/>
+      <pane ySplit="1" topLeftCell="A942" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2946" sqref="A2946"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -79319,6 +79469,972 @@
       </c>
       <c r="H2918" t="s">
         <v>2152</v>
+      </c>
+    </row>
+    <row r="2919" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2919" t="str">
+        <f t="shared" ref="A2919:A2964" si="35">C2919&amp;E2919&amp;G2919</f>
+        <v>cat_vol_multiples_glass_single</v>
+      </c>
+      <c r="B2919" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2919" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2919" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E2919" t="s">
+        <v>2158</v>
+      </c>
+      <c r="H2919" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2920" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2920" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_glass_2_pack</v>
+      </c>
+      <c r="B2920" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2920" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2920" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E2920" t="s">
+        <v>2162</v>
+      </c>
+      <c r="H2920" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2921" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2921" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_glass_3_pack</v>
+      </c>
+      <c r="B2921" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2921" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2921" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E2921" t="s">
+        <v>2163</v>
+      </c>
+      <c r="H2921" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2922" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2922" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_glass_4_pack</v>
+      </c>
+      <c r="B2922" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2922" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2922" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E2922" t="s">
+        <v>2164</v>
+      </c>
+      <c r="H2922" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2923" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2923" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_glass_6_pack</v>
+      </c>
+      <c r="B2923" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2923" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2923" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E2923" t="s">
+        <v>2165</v>
+      </c>
+      <c r="H2923" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2924" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2924" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_glass_8_pack</v>
+      </c>
+      <c r="B2924" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2924" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2924" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E2924" t="s">
+        <v>2166</v>
+      </c>
+      <c r="H2924" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2925" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2925" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_glass_10_pack</v>
+      </c>
+      <c r="B2925" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2925" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2925" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E2925" t="s">
+        <v>2167</v>
+      </c>
+      <c r="H2925" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2926" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2926" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_glass_12_pack</v>
+      </c>
+      <c r="B2926" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2926" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2926" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E2926" t="s">
+        <v>2168</v>
+      </c>
+      <c r="H2926" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2927" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2927" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_glass_15_pack</v>
+      </c>
+      <c r="B2927" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2927" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2927" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E2927" t="s">
+        <v>2169</v>
+      </c>
+      <c r="H2927" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2928" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2928" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_glass_18_pack</v>
+      </c>
+      <c r="B2928" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2928" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2928" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E2928" t="s">
+        <v>2170</v>
+      </c>
+      <c r="H2928" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2929" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2929" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_glass_20_pack</v>
+      </c>
+      <c r="B2929" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2929" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2929" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E2929" t="s">
+        <v>2171</v>
+      </c>
+      <c r="H2929" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2930" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2930" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_glass_24_pack</v>
+      </c>
+      <c r="B2930" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2930" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2930" t="s">
+        <v>2155</v>
+      </c>
+      <c r="E2930" t="s">
+        <v>2172</v>
+      </c>
+      <c r="H2930" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2931" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2931" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_can_single</v>
+      </c>
+      <c r="B2931" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2931" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2931" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2931" t="s">
+        <v>2159</v>
+      </c>
+      <c r="H2931" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2932" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2932" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_can_2_pack</v>
+      </c>
+      <c r="B2932" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2932" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2932" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2932" t="s">
+        <v>2173</v>
+      </c>
+      <c r="H2932" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2933" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2933" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_can_4_pack</v>
+      </c>
+      <c r="B2933" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2933" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2933" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2933" t="s">
+        <v>2174</v>
+      </c>
+      <c r="H2933" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2934" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2934" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_can_6_pack</v>
+      </c>
+      <c r="B2934" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2934" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2934" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2934" t="s">
+        <v>2175</v>
+      </c>
+      <c r="H2934" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2935" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2935" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_can_8_pack</v>
+      </c>
+      <c r="B2935" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2935" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2935" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2935" t="s">
+        <v>2176</v>
+      </c>
+      <c r="H2935" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2936" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2936" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_can_10_pack</v>
+      </c>
+      <c r="B2936" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2936" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2936" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2936" t="s">
+        <v>2177</v>
+      </c>
+      <c r="H2936" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2937" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2937" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_can_12_pack</v>
+      </c>
+      <c r="B2937" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2937" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2937" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2937" t="s">
+        <v>2178</v>
+      </c>
+      <c r="H2937" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2938" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2938" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_can_15_pack</v>
+      </c>
+      <c r="B2938" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2938" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2938" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2938" t="s">
+        <v>2179</v>
+      </c>
+      <c r="H2938" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2939" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2939" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_can_18_pack</v>
+      </c>
+      <c r="B2939" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2939" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2939" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2939" t="s">
+        <v>2180</v>
+      </c>
+      <c r="H2939" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2940" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2940" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_can_20_pack</v>
+      </c>
+      <c r="B2940" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2940" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2940" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2940" t="s">
+        <v>2181</v>
+      </c>
+      <c r="H2940" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2941" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2941" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_multiples_can_24_pack</v>
+      </c>
+      <c r="B2941" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2941" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2941" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2941" t="s">
+        <v>2182</v>
+      </c>
+      <c r="H2941" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2942" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2942" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_glass_single</v>
+      </c>
+      <c r="B2942" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2942" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2942" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E2942" t="s">
+        <v>2160</v>
+      </c>
+      <c r="H2942" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2943" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2943" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_glass_2_pack</v>
+      </c>
+      <c r="B2943" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2943" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2943" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E2943" t="s">
+        <v>2183</v>
+      </c>
+      <c r="H2943" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2944" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2944" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_glass_3_pack</v>
+      </c>
+      <c r="B2944" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2944" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2944" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E2944" t="s">
+        <v>2184</v>
+      </c>
+      <c r="H2944" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2945" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2945" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_glass_4_pack</v>
+      </c>
+      <c r="B2945" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2945" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2945" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E2945" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H2945" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2946" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2946" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_glass_5_pack</v>
+      </c>
+      <c r="B2946" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2946" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2946" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E2946" t="s">
+        <v>2186</v>
+      </c>
+      <c r="H2946" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2947" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2947" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_glass_6_pack</v>
+      </c>
+      <c r="B2947" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2947" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2947" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E2947" t="s">
+        <v>2187</v>
+      </c>
+      <c r="H2947" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2948" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2948" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_glass_10_pack</v>
+      </c>
+      <c r="B2948" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2948" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2948" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E2948" t="s">
+        <v>2188</v>
+      </c>
+      <c r="H2948" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2949" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2949" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_glass_12_pack</v>
+      </c>
+      <c r="B2949" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2949" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2949" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E2949" t="s">
+        <v>2189</v>
+      </c>
+      <c r="H2949" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2950" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2950" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_glass_15_pack</v>
+      </c>
+      <c r="B2950" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2950" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2950" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E2950" t="s">
+        <v>2190</v>
+      </c>
+      <c r="H2950" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2951" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2951" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_glass_8_pack</v>
+      </c>
+      <c r="B2951" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2951" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2951" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E2951" t="s">
+        <v>2191</v>
+      </c>
+      <c r="H2951" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2952" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2952" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_glass_18_pack</v>
+      </c>
+      <c r="B2952" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2952" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2952" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E2952" t="s">
+        <v>2192</v>
+      </c>
+      <c r="H2952" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2953" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2953" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_glass_20_pack</v>
+      </c>
+      <c r="B2953" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2953" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2953" t="s">
+        <v>2157</v>
+      </c>
+      <c r="E2953" t="s">
+        <v>2193</v>
+      </c>
+      <c r="H2953" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2954" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2954" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_can_24_pack</v>
+      </c>
+      <c r="B2954" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2954" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2954" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2954" t="s">
+        <v>2194</v>
+      </c>
+      <c r="H2954" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2955" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2955" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_can_single</v>
+      </c>
+      <c r="B2955" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2955" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2955" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2955" t="s">
+        <v>2161</v>
+      </c>
+      <c r="H2955" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2956" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2956" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_can_4_pack</v>
+      </c>
+      <c r="B2956" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2956" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2956" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2956" t="s">
+        <v>2195</v>
+      </c>
+      <c r="H2956" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2957" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2957" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_can_6_pack</v>
+      </c>
+      <c r="B2957" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2957" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2957" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2957" t="s">
+        <v>2196</v>
+      </c>
+      <c r="H2957" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2958" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2958" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_can_10_pack</v>
+      </c>
+      <c r="B2958" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2958" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2958" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2958" t="s">
+        <v>2197</v>
+      </c>
+      <c r="H2958" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2959" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2959" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_can_12_pack</v>
+      </c>
+      <c r="B2959" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2959" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2959" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2959" t="s">
+        <v>2198</v>
+      </c>
+      <c r="H2959" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2960" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2960" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_can_15_pack</v>
+      </c>
+      <c r="B2960" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2960" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2960" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2960" t="s">
+        <v>2199</v>
+      </c>
+      <c r="H2960" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2961" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2961" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_can_8_pack</v>
+      </c>
+      <c r="B2961" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2961" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2961" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2961" t="s">
+        <v>2200</v>
+      </c>
+      <c r="H2961" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2962" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2962" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_can_18_pack</v>
+      </c>
+      <c r="B2962" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2962" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2962" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2962" t="s">
+        <v>2201</v>
+      </c>
+      <c r="H2962" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2963" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2963" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_can_20_pack</v>
+      </c>
+      <c r="B2963" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2963" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2963" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2963" t="s">
+        <v>2202</v>
+      </c>
+      <c r="H2963" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="2964" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2964" t="str">
+        <f t="shared" si="35"/>
+        <v>cat_vol_impulse_can_24_pack</v>
+      </c>
+      <c r="B2964" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C2964" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D2964" t="s">
+        <v>2156</v>
+      </c>
+      <c r="E2964" t="s">
+        <v>2194</v>
+      </c>
+      <c r="H2964" t="s">
+        <v>2141</v>
       </c>
     </row>
   </sheetData>
@@ -79485,6 +80601,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2B45C0EA743584A8108406922405CD9" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="28eea7f25acf351aeb308c66c2a0cc34">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f859e2c-e6b3-43fd-84f3-2e79f1815da7" xmlns:ns3="af2a5c73-a52b-4877-934f-731a7896a6a0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0c229cfe8c0dd97038f86cb311aeef9c" ns2:_="" ns3:_="">
     <xsd:import namespace="3f859e2c-e6b3-43fd-84f3-2e79f1815da7"/>
@@ -79661,22 +80786,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B5E19E5-20AC-4670-9F44-7E00AC29618F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4BDD481-501C-4200-9B28-7D89CE3D9024}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -79695,19 +80819,11 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C04BD6B-3FF1-42AA-AC81-EB54DE3A1588}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B5E19E5-20AC-4670-9F44-7E00AC29618F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>